<commit_message>
Changing repo name to SiteOps.
</commit_message>
<xml_diff>
--- a/Checklists/CHECKLIST GERAL.xlsx
+++ b/Checklists/CHECKLIST GERAL.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansuenaga/Dev/OpsFESP/Checklists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmmoreira/Google Drive/Tabelas/7 - NbOps/Checklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27320" yWindow="-580" windowWidth="27320" windowHeight="13300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GERAL" sheetId="1" r:id="rId1"/>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,11 +852,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G1" t="s">

</xml_diff>